<commit_message>
Parts and Trailer Catalog scenarios
</commit_message>
<xml_diff>
--- a/src/test/java/DataFiles/PartNames.xlsx
+++ b/src/test/java/DataFiles/PartNames.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">DEF</t>
   </si>
   <si>
-    <t xml:space="preserve">TARP,ROLL OVER,40'X96",ALFC,OTH RC</t>
+    <t xml:space="preserve">Replacement Tarp - 18 oz. Super Duty</t>
   </si>
 </sst>
 </file>
@@ -114,13 +114,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -143,10 +147,10 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -164,7 +168,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>